<commit_message>
update models, delete old files
</commit_message>
<xml_diff>
--- a/incentives/state_scenarios_for_import.xlsx
+++ b/incentives/state_scenarios_for_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/BioLocE/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0646E4-20AF-9841-A469-72CD771103EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD929AB-4C1B-C44D-B72F-2358BB7D3AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>State</t>
   </si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t>Electricity GWP-100 (kg CO2-eq/kWh)</t>
+  </si>
+  <si>
+    <t>CS Price (USD/kg)</t>
+  </si>
+  <si>
+    <t>SC Price (USD/kg)</t>
+  </si>
+  <si>
+    <t>CN Price (USD/kg)</t>
   </si>
 </sst>
 </file>
@@ -610,15 +619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0865C41F-F8C1-F743-9CC7-E8990FCDD1B0}">
-  <dimension ref="A1:P119"/>
+  <dimension ref="A1:Q119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,11 +661,20 @@
       <c r="K1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="5"/>
+      <c r="L1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -687,8 +705,12 @@
       <c r="K2" s="4">
         <v>0.48249069999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -716,11 +738,13 @@
       <c r="K3" s="4">
         <v>0.50515179999999993</v>
       </c>
-      <c r="N3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -748,11 +772,13 @@
       <c r="K4" s="4">
         <v>0.65622580000000008</v>
       </c>
-      <c r="N4" s="5"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -780,11 +806,15 @@
       <c r="K5" s="4">
         <v>0.48249069999999999</v>
       </c>
-      <c r="N5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4">
+        <v>0.1</v>
+      </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -812,11 +842,15 @@
       <c r="K6" s="4">
         <v>0.61090359999999999</v>
       </c>
-      <c r="N6" s="5"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
+        <v>9.9000000000000005E-2</v>
+      </c>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -847,11 +881,15 @@
       <c r="K7" s="4">
         <v>0.63356469999999998</v>
       </c>
-      <c r="N7" s="5"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
+        <v>0.10100000000000001</v>
+      </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -879,11 +917,13 @@
       <c r="K8" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="N8" s="5"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -911,11 +951,15 @@
       <c r="K9" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="N9" s="5"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4">
+        <v>0.107</v>
+      </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -943,11 +987,18 @@
       <c r="K10" s="4">
         <v>0.474937</v>
       </c>
-      <c r="N10" s="5"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="N10" s="4">
+        <v>4.0454826894677567E-2</v>
+      </c>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -975,11 +1026,15 @@
       <c r="K11" s="4">
         <v>0.474937</v>
       </c>
-      <c r="N11" s="5"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4">
+        <v>0.1</v>
+      </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1010,11 +1065,16 @@
       <c r="K12" s="4">
         <v>0.50515179999999993</v>
       </c>
-      <c r="N12" s="5"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4">
+        <v>4.4864072332789565E-2</v>
+      </c>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1042,11 +1102,13 @@
       <c r="K13" s="4">
         <v>0.55802770000000002</v>
       </c>
-      <c r="N13" s="5"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1074,11 +1136,15 @@
       <c r="K14" s="4">
         <v>0.55802770000000002</v>
       </c>
-      <c r="N14" s="5"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4">
+        <v>9.9000000000000005E-2</v>
+      </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1106,11 +1172,15 @@
       <c r="K15" s="4">
         <v>0.57313510000000001</v>
       </c>
-      <c r="N15" s="5"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4">
+        <v>0.1</v>
+      </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1141,11 +1211,15 @@
       <c r="K16" s="4">
         <v>0.56558140000000001</v>
       </c>
-      <c r="N16" s="5"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1176,11 +1250,15 @@
       <c r="K17" s="4">
         <v>0.67133320000000007</v>
       </c>
-      <c r="N17" s="5"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4">
+        <v>9.2999999999999999E-2</v>
+      </c>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1211,11 +1289,15 @@
       <c r="K18" s="4">
         <v>0.49004439999999999</v>
       </c>
-      <c r="N18" s="5"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1246,11 +1328,18 @@
       <c r="K19" s="4">
         <v>0.474937</v>
       </c>
-      <c r="N19" s="5"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="N19" s="4">
+        <v>4.6407308236128764E-2</v>
+      </c>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1278,11 +1367,13 @@
       <c r="K20" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="N20" s="5"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1310,11 +1401,15 @@
       <c r="K21" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="N21" s="5"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1342,11 +1437,13 @@
       <c r="K22" s="4">
         <v>0.474937</v>
       </c>
-      <c r="N22" s="5"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1377,11 +1474,15 @@
       <c r="K23" s="4">
         <v>0.50515179999999993</v>
       </c>
-      <c r="N23" s="5"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4">
+        <v>0.10299999999999999</v>
+      </c>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1409,11 +1510,15 @@
       <c r="K24" s="4">
         <v>0.52781290000000003</v>
       </c>
-      <c r="N24" s="5"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1441,11 +1546,15 @@
       <c r="K25" s="4">
         <v>0.53536660000000003</v>
       </c>
-      <c r="N25" s="5"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1473,11 +1582,15 @@
       <c r="K26" s="4">
         <v>0.57313510000000001</v>
       </c>
-      <c r="N26" s="5"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4">
+        <v>9.0999999999999998E-2</v>
+      </c>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1508,8 +1621,10 @@
       <c r="K27" s="4">
         <v>0.56558140000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1540,8 +1655,12 @@
       <c r="K28" s="4">
         <v>0.61090359999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L28" s="4"/>
+      <c r="M28" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1569,8 +1688,10 @@
       <c r="K29" s="4">
         <v>0.54292030000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1598,8 +1719,10 @@
       <c r="K30" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1627,8 +1750,12 @@
       <c r="K31" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L31" s="4"/>
+      <c r="M31" s="4">
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1659,8 +1786,10 @@
       <c r="K32" s="4">
         <v>0.64867209999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1688,8 +1817,12 @@
       <c r="K33" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" s="4"/>
+      <c r="M33" s="4">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1717,8 +1850,12 @@
       <c r="K34" s="4">
         <v>0.474937</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="4"/>
+      <c r="M34" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1746,8 +1883,12 @@
       <c r="K35" s="4">
         <v>0.56558140000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="4"/>
+      <c r="M35" s="4">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1775,8 +1916,12 @@
       <c r="K36" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" s="4"/>
+      <c r="M36" s="4">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1804,8 +1949,12 @@
       <c r="K37" s="4">
         <v>0.5882425</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" s="4"/>
+      <c r="M37" s="4">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1836,8 +1985,10 @@
       <c r="K38" s="4">
         <v>0.54292030000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1865,8 +2016,12 @@
       <c r="K39" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" s="4"/>
+      <c r="M39" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1894,8 +2049,10 @@
       <c r="K40" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1926,8 +2083,12 @@
       <c r="K41" s="4">
         <v>0.474937</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" s="4"/>
+      <c r="M41" s="4">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1955,8 +2116,12 @@
       <c r="K42" s="4">
         <v>0.55047400000000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" s="4"/>
+      <c r="M42" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1984,8 +2149,12 @@
       <c r="K43" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43" s="4"/>
+      <c r="M43" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2013,8 +2182,15 @@
       <c r="K44" s="4">
         <v>0.52781290000000003</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44" s="4"/>
+      <c r="M44" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="N44" s="4">
+        <v>2.1495071510795983E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2045,8 +2221,10 @@
       <c r="K45" s="4">
         <v>0.51270550000000004</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2074,8 +2252,10 @@
       <c r="K46" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2106,8 +2286,12 @@
       <c r="K47" s="4">
         <v>0.48249069999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47" s="4"/>
+      <c r="M47" s="4">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2135,8 +2319,10 @@
       <c r="K48" s="4">
         <v>0.56558140000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2164,8 +2350,12 @@
       <c r="K49" s="4">
         <v>0.4673833</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" s="4"/>
+      <c r="M49" s="4">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2193,8 +2383,12 @@
       <c r="K50" s="4">
         <v>0.56558140000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50" s="4"/>
+      <c r="M50" s="4">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2222,16 +2416,17 @@
       <c r="K51" s="4">
         <v>0.48249069999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F54" s="3"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -2388,8 +2583,8 @@
       <c r="B119" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:P26">
-    <sortCondition ref="P3:P26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O3:Q26">
+    <sortCondition ref="Q3:Q26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>